<commit_message>
Se modifican Locators, Autenticacion, redacción y question de diferentes transacciones
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/billetera/RegistroBilletera.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/billetera/RegistroBilletera.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\OSP_NEW\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\autenticacion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695"/>
+    <workbookView windowWidth="20490" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -64,7 +59,7 @@
     <t>1037655531</t>
   </si>
   <si>
-    <t>userqa10</t>
+    <t>userrobot3</t>
   </si>
   <si>
     <t>1234</t>
@@ -137,34 +132,19 @@
   </si>
   <si>
     <t>Consultas</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>1111</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>95400152</t>
-  </si>
-  <si>
-    <t>sandrita69</t>
-  </si>
-  <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>0370</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -180,21 +160,158 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,8 +330,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -237,33 +540,318 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="Normal 2" xfId="32"/>
+    <cellStyle name="20% - Accent5" xfId="33" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="34" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="35" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="36" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="38" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="39" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="40" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="41" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="42" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="43" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="44" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="45" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="46" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="47" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="48" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="49" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -521,26 +1109,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="11.125" customWidth="1"/>
     <col min="2" max="6" width="14.375" customWidth="1"/>
     <col min="9" max="9" width="18.375" customWidth="1"/>
     <col min="10" max="10" width="22.125" customWidth="1"/>
     <col min="11" max="11" width="14.375" customWidth="1"/>
-    <col min="12" max="12" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -619,109 +1207,28 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:J2">
+      <formula1>Listas!$A$2:$A$3</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Listas!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:J4</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="10.625" customWidth="1"/>
     <col min="2" max="2" width="14.875" customWidth="1"/>
@@ -771,7 +1278,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="2:4">
       <c r="B4" t="s">
         <v>34</v>
       </c>
@@ -779,22 +1286,23 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="2:2">
       <c r="B5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="2:2">
       <c r="B6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="2:2">
       <c r="B7" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactorización clase general page, se agrega el target generico BTN_PERMISO, el cual otorga permisos sobre camara y llamadas en el dispositivo
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/billetera/RegistroBilletera.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/billetera/RegistroBilletera.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOPS\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\billetera\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88781C26-87B3-470E-B951-7BF6BDECC811}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3823D12F-BE4F-4B68-8817-99E810DDD30B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -134,7 +134,7 @@
     <t>Consultas</t>
   </si>
   <si>
-    <t>autotest10</t>
+    <t>autotest12</t>
   </si>
 </sst>
 </file>
@@ -502,7 +502,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5"/>
@@ -558,7 +558,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="7">
-        <v>67652517</v>
+        <v>48349402</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>12</v>

</xml_diff>